<commit_message>
Add Fixed/Variable modification to assay.isa.xlsx
</commit_message>
<xml_diff>
--- a/assays/proteomicsTemplate/assay.template/assay.isa.xlsx
+++ b/assays/proteomicsTemplate/assay.template/assay.isa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mauso\Google Drive\CSB-Stuff\NFDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\ARC\assays\proteomicsTemplate\assay.template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE2FECC-C148-472A-80E5-07599020C7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5221A347-2EC8-4644-B8DF-3FF43922AFE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{B0FB3F19-C527-41AF-B02D-0669FBE7650F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B0FB3F19-C527-41AF-B02D-0669FBE7650F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample preparation" sheetId="1" r:id="rId1"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
   <si>
     <t>Source Name</t>
   </si>
@@ -590,6 +590,24 @@
   </si>
   <si>
     <t>(original in sample sheet)</t>
+  </si>
+  <si>
+    <t>Parameter [Fixed modification]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Fixed modification] (#h)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Fixed modification] (#h)</t>
+  </si>
+  <si>
+    <t>Parameter [Variable modification]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Variable modification] (#h)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Variable modification] (#h)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +696,13 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
@@ -790,64 +814,64 @@
   <autoFilter ref="A2:BI3" xr:uid="{A021418B-0175-4598-91AE-1DE7C5AC79BB}"/>
   <tableColumns count="61">
     <tableColumn id="1" xr3:uid="{32B5DD65-5DA9-4472-A9B2-CBD1DA288E9D}" name="Source Name"/>
-    <tableColumn id="2" xr3:uid="{0051F93D-5B57-4B19-B3D9-4C0CB04ACCB8}" name="Characteristics [organism or virus or viroid]" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{0051F93D-5B57-4B19-B3D9-4C0CB04ACCB8}" name="Characteristics [organism or virus or viroid]" dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{7D8276DB-7065-4D96-A647-97FE0DE02368}" name="Term Source REF [organism or virus or viroid] (#h)"/>
     <tableColumn id="4" xr3:uid="{D99FCE4D-D5E6-488A-8DFC-3D06ED543DC0}" name="Term Accession Number [organism or virus or viroid] (#h)"/>
-    <tableColumn id="5" xr3:uid="{3A2A4C8E-56AC-422D-992B-F0EB6AE36DB2}" name="Characteristics [genetic experimental form]" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{3A2A4C8E-56AC-422D-992B-F0EB6AE36DB2}" name="Characteristics [genetic experimental form]" dataDxfId="31"/>
     <tableColumn id="6" xr3:uid="{8C5CEA4B-6B30-4C92-A357-EAB9E6C92F49}" name="Term Source REF [genetic experimental form] (#h)"/>
     <tableColumn id="7" xr3:uid="{F2BDA43D-D8EA-4B2A-AE9B-257C43E1814A}" name="Term Accession Number [genetic experimental form] (#h)"/>
-    <tableColumn id="8" xr3:uid="{483328BD-F981-4D5F-911B-C8D6030CB53C}" name="Characteristics [experimental preparation]" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{483328BD-F981-4D5F-911B-C8D6030CB53C}" name="Characteristics [experimental preparation]" dataDxfId="30"/>
     <tableColumn id="9" xr3:uid="{64F403CD-137A-4C5C-B371-45F2C78B8640}" name="Term Source REF [experimental preparation] (#h)"/>
     <tableColumn id="10" xr3:uid="{9AAC3412-A570-463A-AA0C-4CEEA5C55D12}" name="Term Accession Number [experimental preparation] (#h)"/>
-    <tableColumn id="11" xr3:uid="{723BACD2-2250-4CCA-B64D-7B8B0455D0AB}" name="Characteristics [tag]" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{723BACD2-2250-4CCA-B64D-7B8B0455D0AB}" name="Characteristics [tag]" dataDxfId="29"/>
     <tableColumn id="12" xr3:uid="{49BAE384-9089-439A-8EB0-B88AFF35E812}" name="Term Source REF [tag] (#h)"/>
     <tableColumn id="13" xr3:uid="{62260698-533D-426F-AF92-550F431BB799}" name="Term Accession Number [tag] (#h)"/>
-    <tableColumn id="14" xr3:uid="{C02B08BC-EEC9-4500-BB3E-9EB8240F4E72}" name="Characteristics [Biospecimen]" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{C02B08BC-EEC9-4500-BB3E-9EB8240F4E72}" name="Characteristics [Biospecimen]" dataDxfId="28"/>
     <tableColumn id="15" xr3:uid="{D9F9C48D-E61D-4520-BC12-5F73A9700CD9}" name="Term Source REF [Biospecimen] (#h)"/>
     <tableColumn id="16" xr3:uid="{4BB2D42E-F79D-4149-A474-F4270E07F4F8}" name="Term Accession Number [Biospecimen] (#h)"/>
-    <tableColumn id="17" xr3:uid="{96D91E84-F99F-46D7-A050-C4DD36C14D82}" name="Characteristics [biological replicate]" dataDxfId="25"/>
+    <tableColumn id="17" xr3:uid="{96D91E84-F99F-46D7-A050-C4DD36C14D82}" name="Characteristics [biological replicate]" dataDxfId="27"/>
     <tableColumn id="18" xr3:uid="{2B7ABA4B-5463-4308-891D-C9E06828AFF2}" name="Term Source REF [biological replicate] (#h)"/>
     <tableColumn id="19" xr3:uid="{46464C16-8A80-4A59-BD5E-65E0776552C0}" name="Term Accession Number [biological replicate] (#h)"/>
-    <tableColumn id="32" xr3:uid="{8264F1BE-3D5D-43D3-B868-09496276DCAA}" name="Parameter [sample process]" dataDxfId="24"/>
+    <tableColumn id="32" xr3:uid="{8264F1BE-3D5D-43D3-B868-09496276DCAA}" name="Parameter [sample process]" dataDxfId="26"/>
     <tableColumn id="33" xr3:uid="{E8BF7436-8C63-4B76-8A56-01F61086FC80}" name="Term Source REF [sample process] (#h)"/>
     <tableColumn id="34" xr3:uid="{913F3EAA-125B-4197-84BE-DD725F669D71}" name="Term Accession Number [sample process] (#h)"/>
-    <tableColumn id="35" xr3:uid="{0A8CA8A0-F698-4643-8902-8D971B9FF318}" name="Parameter [matrix solution]" dataDxfId="23"/>
+    <tableColumn id="35" xr3:uid="{0A8CA8A0-F698-4643-8902-8D971B9FF318}" name="Parameter [matrix solution]" dataDxfId="25"/>
     <tableColumn id="36" xr3:uid="{5423C338-503E-4F29-843C-1CA1DD10EF65}" name="Term Source REF [matrix solution] (#h)"/>
     <tableColumn id="37" xr3:uid="{28064116-BEC0-4F75-BD2B-79FB7DE79276}" name="Term Accession Number [matrix solution] (#h)"/>
-    <tableColumn id="38" xr3:uid="{D5A602F7-BB81-47F7-B2E2-7830A27F5C97}" name="Parameter [cleavage agent name]" dataDxfId="22"/>
+    <tableColumn id="38" xr3:uid="{D5A602F7-BB81-47F7-B2E2-7830A27F5C97}" name="Parameter [cleavage agent name]" dataDxfId="24"/>
     <tableColumn id="39" xr3:uid="{576B5F5F-B9EF-464A-91B5-008DD42CF3E1}" name="Term Source REF [cleavage agent name] (#h)"/>
     <tableColumn id="40" xr3:uid="{D4024777-8B34-476A-850C-215A85B91755}" name="Term Accession Number [cleavage agent name] (#h)"/>
-    <tableColumn id="41" xr3:uid="{C283EF53-C3E8-4C3F-9AEA-9909640B4C6B}" name="Parameter [molecule]" dataDxfId="21"/>
+    <tableColumn id="41" xr3:uid="{C283EF53-C3E8-4C3F-9AEA-9909640B4C6B}" name="Parameter [molecule]" dataDxfId="23"/>
     <tableColumn id="42" xr3:uid="{17806147-4679-4175-A692-CB0C7311F23C}" name="Term Source REF [molecule] (#h)"/>
     <tableColumn id="43" xr3:uid="{1A9D0196-A75C-4466-8D09-8C6FD5F77826}" name="Term Accession Number [molecule] (#h)"/>
-    <tableColumn id="44" xr3:uid="{B62B84F2-F16E-4311-AE97-C192785B6BB8}" name="Parameter [sample state]" dataDxfId="20"/>
+    <tableColumn id="44" xr3:uid="{B62B84F2-F16E-4311-AE97-C192785B6BB8}" name="Parameter [sample state]" dataDxfId="22"/>
     <tableColumn id="45" xr3:uid="{31379BD3-8C60-4A1E-A859-E73EADE614EA}" name="Term Source REF [sample state] (#h)"/>
     <tableColumn id="46" xr3:uid="{5533A44B-49AF-4230-8CF7-8DFDD5F684E0}" name="Term Accession Number [sample state] (#h)"/>
-    <tableColumn id="47" xr3:uid="{C14A434B-9183-4AB9-911D-8AA11DAF9378}" name="Parameter [multidimensional protein identification technology]" dataDxfId="19"/>
+    <tableColumn id="47" xr3:uid="{C14A434B-9183-4AB9-911D-8AA11DAF9378}" name="Parameter [multidimensional protein identification technology]" dataDxfId="21"/>
     <tableColumn id="48" xr3:uid="{043A2D11-A8AC-4877-A111-9BFEBBC9F8D4}" name="Term Source REF [multidimensional protein identification technology] (#h)"/>
     <tableColumn id="49" xr3:uid="{8F8BB5F4-3D57-49DE-8BFF-17F7447798B6}" name="Term Accession Number [multidimensional protein identification technology] (#h)"/>
-    <tableColumn id="50" xr3:uid="{875313D9-4DB3-409C-8E51-6BE0646CC36B}" name="Parameter [molecular weight estimation by staining]" dataDxfId="18"/>
+    <tableColumn id="50" xr3:uid="{875313D9-4DB3-409C-8E51-6BE0646CC36B}" name="Parameter [molecular weight estimation by staining]" dataDxfId="20"/>
     <tableColumn id="51" xr3:uid="{8F5FB22E-D2FA-4211-9847-A5408E04E75D}" name="Term Source REF [molecular weight estimation by staining] (#h)"/>
     <tableColumn id="52" xr3:uid="{229F37A0-15A4-4B36-B1D8-877A059CA387}" name="Term Accession Number [molecular weight estimation by staining] (#h)"/>
-    <tableColumn id="53" xr3:uid="{AC0CB339-EA5B-4687-A874-332ED311B6AD}" name="Parameter [buffer]" dataDxfId="17"/>
+    <tableColumn id="53" xr3:uid="{AC0CB339-EA5B-4687-A874-332ED311B6AD}" name="Parameter [buffer]" dataDxfId="19"/>
     <tableColumn id="54" xr3:uid="{B2A6EE1D-7A15-4ED2-8898-EC2481F63301}" name="Term Source REF [buffer] (#h)"/>
     <tableColumn id="55" xr3:uid="{877F55DC-7840-4F5B-B5B5-34389A151DEC}" name="Term Accession Number [buffer] (#h)"/>
-    <tableColumn id="56" xr3:uid="{D169A25A-7B94-4042-8E00-AF7CEE8F4509}" name="Parameter [pH]" dataDxfId="16"/>
+    <tableColumn id="56" xr3:uid="{D169A25A-7B94-4042-8E00-AF7CEE8F4509}" name="Parameter [pH]" dataDxfId="18"/>
     <tableColumn id="57" xr3:uid="{2925FFD0-6029-4071-B7B2-353D534D211C}" name="Term Source REF [pH] (#h)"/>
     <tableColumn id="58" xr3:uid="{98F07EB2-7EC9-4C54-8FB0-6806B27ECBF3}" name="Term Accession Number [pH] (#h)"/>
-    <tableColumn id="74" xr3:uid="{21DDD859-2FA7-4E76-9CD7-513290E68863}" name="Parameter [chromatography separation]" dataDxfId="15"/>
+    <tableColumn id="74" xr3:uid="{21DDD859-2FA7-4E76-9CD7-513290E68863}" name="Parameter [chromatography separation]" dataDxfId="17"/>
     <tableColumn id="75" xr3:uid="{EC43C1CC-1C7B-4676-B0E5-D55D848E54E4}" name="Term Source REF [chromatography separation] (#h)"/>
     <tableColumn id="76" xr3:uid="{AE3F3130-AB79-402E-AE33-2EE62E1385CA}" name="Term Accession Number [chromatography separation] (#h)"/>
-    <tableColumn id="59" xr3:uid="{8BE99A3A-FA34-4DD9-9650-6F887D44155B}" name="Parameter [sample desalting]" dataDxfId="14"/>
+    <tableColumn id="59" xr3:uid="{8BE99A3A-FA34-4DD9-9650-6F887D44155B}" name="Parameter [sample desalting]" dataDxfId="16"/>
     <tableColumn id="60" xr3:uid="{66E5FB66-5AEC-4B74-85F9-F9AD3A06D9BD}" name="Term Source REF [sample desalting] (#h)"/>
     <tableColumn id="61" xr3:uid="{8ACF1992-7314-4CAA-8A52-06CDBC1B5CCC}" name="Term Accession Number [sample desalting] (#h)"/>
-    <tableColumn id="65" xr3:uid="{CEA9E2E4-6E80-4512-B643-84895199F4F0}" name="Parameter [temperature]" dataDxfId="13"/>
+    <tableColumn id="65" xr3:uid="{CEA9E2E4-6E80-4512-B643-84895199F4F0}" name="Parameter [temperature]" dataDxfId="15"/>
     <tableColumn id="66" xr3:uid="{226BBDC8-1C97-4A38-A75F-9BE1523DE4AA}" name="Term Source REF [temperature] (#h)"/>
     <tableColumn id="67" xr3:uid="{C043710B-81D1-46AD-A58F-C8925C7FFE3F}" name="Term Accession Number [temperature] (#h)"/>
-    <tableColumn id="68" xr3:uid="{B222FC6F-EEE2-4F7E-BC9D-F81EB938C59B}" name="Parameter [time]" dataDxfId="12"/>
+    <tableColumn id="68" xr3:uid="{B222FC6F-EEE2-4F7E-BC9D-F81EB938C59B}" name="Parameter [time]" dataDxfId="14"/>
     <tableColumn id="69" xr3:uid="{A32B46CF-3E77-43C2-AF3E-B6F72F661A9F}" name="Term Source REF [time] (#h)"/>
     <tableColumn id="70" xr3:uid="{9C83C43B-F36C-4DBA-B68D-B8FD6CCFD28E}" name="Term Accession Number [time] (#h)"/>
-    <tableColumn id="71" xr3:uid="{3ED698DD-B3FA-40D4-B36C-F69D948D0E38}" name="Sample Name" dataDxfId="11"/>
+    <tableColumn id="71" xr3:uid="{3ED698DD-B3FA-40D4-B36C-F69D948D0E38}" name="Sample Name" dataDxfId="13"/>
     <tableColumn id="72" xr3:uid="{36B73D20-FD95-491C-9E58-1F6DD64E0F18}" name="Term Source REF [Sample Name] (#h)"/>
     <tableColumn id="73" xr3:uid="{600BEF04-64C1-42EF-A5E7-567F6410A4E2}" name="Term Accession Number [Sample Name] (#h)"/>
   </tableColumns>
@@ -856,29 +880,35 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F8C55CE-8442-4239-AE2E-8C50EF28E697}" name="annotationTable1" displayName="annotationTable1" ref="A2:V3" totalsRowShown="0">
-  <autoFilter ref="A2:V3" xr:uid="{AE348682-3FEE-4C09-AC04-24C93DD236EB}"/>
-  <tableColumns count="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9F8C55CE-8442-4239-AE2E-8C50EF28E697}" name="annotationTable1" displayName="annotationTable1" ref="A2:AB3" totalsRowShown="0">
+  <autoFilter ref="A2:AB3" xr:uid="{AE348682-3FEE-4C09-AC04-24C93DD236EB}"/>
+  <tableColumns count="28">
     <tableColumn id="1" xr3:uid="{101E48DE-3613-4B20-9747-32443B12E1CF}" name="Source Name"/>
-    <tableColumn id="2" xr3:uid="{E0989224-D939-4CE6-9519-15C0EF3EB009}" name="Parameter [technical replicate]" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E0989224-D939-4CE6-9519-15C0EF3EB009}" name="Parameter [technical replicate]" dataDxfId="12"/>
     <tableColumn id="3" xr3:uid="{0BFA3805-B56A-4639-ADB5-09A7259936E9}" name="Term Source REF [technical replicate] (#h)"/>
     <tableColumn id="4" xr3:uid="{668476C9-5075-4802-868D-3AE5B26DD7B8}" name="Term Accession Number [technical replicate] (#h)"/>
-    <tableColumn id="5" xr3:uid="{910812ED-83B8-4970-AA10-79F93CDE3A22}" name="Parameter [sample volume]" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{6A2FBD19-0A27-4583-B0B0-C99D8D6E5CA1}" name="Parameter [Variable modification]" dataDxfId="0"/>
+    <tableColumn id="27" xr3:uid="{11359F1F-6C13-4C48-91EF-7BA2ECA42553}" name="Term Source REF [Variable modification] (#h)"/>
+    <tableColumn id="28" xr3:uid="{0F92F580-500C-4139-9981-41B14237DFB2}" name="Term Accession Number [Variable modification] (#h)"/>
+    <tableColumn id="23" xr3:uid="{545210EC-E8D4-4743-A2BA-6FC7795EDBAF}" name="Parameter [Fixed modification]" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{64B89B08-8F9C-48FD-A3A8-D4020026022E}" name="Term Source REF [Fixed modification] (#h)"/>
+    <tableColumn id="25" xr3:uid="{D7EAC3CF-125B-4923-913A-097B88B849DD}" name="Term Accession Number [Fixed modification] (#h)"/>
+    <tableColumn id="5" xr3:uid="{910812ED-83B8-4970-AA10-79F93CDE3A22}" name="Parameter [sample volume]" dataDxfId="11"/>
     <tableColumn id="6" xr3:uid="{1EA11368-ECD8-4E4C-AF08-C0DC937B9D92}" name="Term Source REF [sample volume] (#h)"/>
     <tableColumn id="7" xr3:uid="{1BF12B47-4164-4D70-908B-9C0F2BA2C1C4}" name="Term Accession Number [sample volume] (#h)"/>
-    <tableColumn id="8" xr3:uid="{EBD53FF8-EF1B-440B-8E4A-2385FA078F77}" name="Parameter [injection volume]" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{EBD53FF8-EF1B-440B-8E4A-2385FA078F77}" name="Parameter [injection volume]" dataDxfId="10"/>
     <tableColumn id="9" xr3:uid="{76E74CBB-C863-4F23-ABFB-5C35279610D6}" name="Term Source REF [injection volume] (#h)"/>
     <tableColumn id="10" xr3:uid="{82F8A8CC-11AA-42A3-910D-04B64DCF31E2}" name="Term Accession Number [injection volume] (#h)"/>
-    <tableColumn id="11" xr3:uid="{F9C8AF4A-2543-4B4C-8AD4-5BBCEED48F26}" name="Parameter [count unit]" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{F9C8AF4A-2543-4B4C-8AD4-5BBCEED48F26}" name="Parameter [count unit]" dataDxfId="9"/>
     <tableColumn id="12" xr3:uid="{23B9BD72-C914-4E18-908D-49291B4E08D1}" name="Term Source REF [count unit] (#h)"/>
     <tableColumn id="13" xr3:uid="{69F77E6E-6DBC-4024-B3D0-FEA0C81CF94A}" name="Term Accession Number [count unit] (#h)"/>
-    <tableColumn id="14" xr3:uid="{2531B27F-A3D7-4BC3-9AD0-D6925C89014B}" name="Parameter [instrument model]" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{2531B27F-A3D7-4BC3-9AD0-D6925C89014B}" name="Parameter [instrument model]" dataDxfId="8"/>
     <tableColumn id="15" xr3:uid="{5047CB43-A1A0-4F0E-A6A1-59ECD77C8EBB}" name="Term Source REF [instrument model] (#h)"/>
     <tableColumn id="16" xr3:uid="{51EACAF8-1B83-40B5-A03E-5170813268F0}" name="Term Accession Number [instrument model] (#h)"/>
-    <tableColumn id="17" xr3:uid="{F6316696-5605-4B74-A958-FA6EAAF3E73D}" name="Parameter [LC-Gradiant]" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{F6316696-5605-4B74-A958-FA6EAAF3E73D}" name="Parameter [LC-Gradiant]" dataDxfId="7"/>
     <tableColumn id="18" xr3:uid="{3371DE6D-49CE-4168-9F9B-424D9BAA297B}" name="Term Source REF [LC-Gradiant] (#h)"/>
     <tableColumn id="19" xr3:uid="{7C70F0B5-C695-4CD2-980C-3CD09DABBA82}" name="Term Accession Number [LC-Gradiant] (#h)"/>
-    <tableColumn id="20" xr3:uid="{EE8BE02C-9304-4030-A53D-0B90FCD9F6CC}" name="Sample Name" dataDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{EE8BE02C-9304-4030-A53D-0B90FCD9F6CC}" name="Sample Name" dataDxfId="6"/>
     <tableColumn id="21" xr3:uid="{13658F18-04EE-436F-AE2E-D6F45207E72C}" name="Term Source REF [Sample Name] (#h)"/>
     <tableColumn id="22" xr3:uid="{9F910BCE-11F1-4374-BF0D-8B475C2D6BA3}" name="Term Accession Number [Sample Name] (#h)"/>
   </tableColumns>
@@ -891,16 +921,16 @@
   <autoFilter ref="A2:M3" xr:uid="{C68BD143-D079-414B-8930-282765795081}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{B6570D44-1FC8-45CE-81D6-945F48269C62}" name="Source Name"/>
-    <tableColumn id="2" xr3:uid="{6B0C1A4E-4D8A-4E9A-9B28-83B8094787D7}" name="Parameter [acquisition software]" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{6B0C1A4E-4D8A-4E9A-9B28-83B8094787D7}" name="Parameter [acquisition software]" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{C31A64FE-1487-4313-B868-72E5255F8DDA}" name="Term Source REF [acquisition software] (#h)"/>
     <tableColumn id="4" xr3:uid="{250209DB-B75E-410A-9925-C1269107AE95}" name="Term Accession Number [acquisition software] (#h)"/>
-    <tableColumn id="5" xr3:uid="{B0E78132-CEC9-4BE8-92A8-FF92DE8E1612}" name="Parameter [analysis software]" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{B0E78132-CEC9-4BE8-92A8-FF92DE8E1612}" name="Parameter [analysis software]" dataDxfId="4"/>
     <tableColumn id="6" xr3:uid="{F9DC585F-C5C8-4D59-B88B-345DFE4CDBC5}" name="Term Source REF [analysis software] (#h)"/>
     <tableColumn id="7" xr3:uid="{6B976B60-21B8-4DBC-8106-BE0AF7CB24B3}" name="Term Accession Number [analysis software] (#h)"/>
-    <tableColumn id="8" xr3:uid="{55686F24-99A3-4023-A93B-3E887AD06EAC}" name="Parameter [data-processing]" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{55686F24-99A3-4023-A93B-3E887AD06EAC}" name="Parameter [data-processing]" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{AE31F26E-3B42-476D-B61C-85B641DB5797}" name="Term Source REF [data-processing] (#h)"/>
     <tableColumn id="10" xr3:uid="{E056DC42-9426-4701-8CC5-39DC383BFD95}" name="Term Accession Number [data-processing] (#h)"/>
-    <tableColumn id="11" xr3:uid="{7BEB4FC3-01E7-4AD4-8499-3F321669A0D6}" name="Sample Name" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{7BEB4FC3-01E7-4AD4-8499-3F321669A0D6}" name="Sample Name" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{387CBD60-77A2-4074-9EE2-51E878193982}" name="Term Source REF [Sample Name] (#h)"/>
     <tableColumn id="13" xr3:uid="{B39BB906-0764-4590-8458-79B9AC0A8418}" name="Term Accession Number [Sample Name] (#h)"/>
   </tableColumns>
@@ -1205,7 +1235,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
+  <wetp:taskpane dockstate="right" visibility="0" width="529" row="4">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1225,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BDD90-A88D-453F-9DD4-25C4532FB6E9}">
   <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1575,9 +1605,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1EE2786-4482-49AF-B030-E3AA2BEBA6BD}">
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
@@ -1588,50 +1618,62 @@
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="45" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="46.42578125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="33.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="40.28515625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.42578125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="47.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.7109375" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="41.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36.5703125" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="43.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="48" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="45" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.42578125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="40.28515625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="40.42578125" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="47.42578125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.7109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="41.7109375" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="36.5703125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="43.5703125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>90</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1645,74 +1687,95 @@
         <v>60</v>
       </c>
       <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" t="s">
+        <v>114</v>
+      </c>
+      <c r="J2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" t="s">
         <v>62</v>
       </c>
-      <c r="G2" t="s">
+      <c r="M2" t="s">
         <v>63</v>
       </c>
-      <c r="H2" t="s">
+      <c r="N2" t="s">
         <v>64</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>65</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
         <v>66</v>
       </c>
-      <c r="K2" t="s">
+      <c r="Q2" t="s">
         <v>67</v>
       </c>
-      <c r="L2" t="s">
+      <c r="R2" t="s">
         <v>68</v>
       </c>
-      <c r="M2" t="s">
+      <c r="S2" t="s">
         <v>69</v>
       </c>
-      <c r="N2" t="s">
+      <c r="T2" t="s">
         <v>70</v>
       </c>
-      <c r="O2" t="s">
+      <c r="U2" t="s">
         <v>71</v>
       </c>
-      <c r="P2" t="s">
+      <c r="V2" t="s">
         <v>72</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="W2" t="s">
         <v>73</v>
       </c>
-      <c r="R2" t="s">
+      <c r="X2" t="s">
         <v>74</v>
       </c>
-      <c r="S2" t="s">
+      <c r="Y2" t="s">
         <v>75</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Z2" t="s">
         <v>55</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>56</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AB2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="E3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="K3" s="1"/>
-      <c r="N3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="K3" s="4"/>
+      <c r="N3" s="4"/>
       <c r="Q3" s="1"/>
       <c r="T3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="Z3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>